<commit_message>
Update: Read only today's emails and restructure template layout
</commit_message>
<xml_diff>
--- a/download_email/email_download_log.xlsx
+++ b/download_email/email_download_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,76 +562,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Completed Extruder Enquiry Form</t>
+          <t>Project Documents: TSE Enquiry and Quotation for Review</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>197a29ce75d667e9</t>
+          <t>197c45252cdeeb84</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>197a29ce75d667e9</t>
+          <t>197c45252cdeeb84</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ahana_git _hub &lt;ahanagithub@gmail.com&gt;</t>
+          <t>Kumar &lt;kum4r18@gmail.com&gt;</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45837.78603009259</v>
+        <v>45839.54337962963</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45837.78603009259</v>
+        <v>45839.54337962963</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45837.78603009259</v>
+        <v>45839.54337962963</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45837.78603009259</v>
+        <v>45839.54337962963</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>enquiry_20250629_185150_TSE enquiry (Ningbo Licheng, Mega50).pdf,enquiry_20250629_185152_Enquiry form - Gulf Additives (Revised 11112024).pdf,enquiry_20250629_185153_Enquiry_form.pdf</t>
+          <t>quotation_20250701_130227_TSE Enquiry form-Mega 80S.pdf, quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/enquiry_20250629_185150_TSE enquiry (Ningbo Licheng, Mega50).pdf,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/enquiry_20250629_185152_Enquiry form - Gulf Additives (Revised 11112024).pdf,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/enquiry_20250629_185153_Enquiry_form.pdf</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250701_130227_TSE Enquiry form-Mega 80S.pdf, /mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/enquiry_20250629_185150_TSE enquiry (Ningbo Licheng, Mega50).json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/enquiry_20250629_185152_Enquiry form - Gulf Additives (Revised 11112024).json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/enquiry_20250629_185153_Enquiry_form.json</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250701_130227_TSE Enquiry form-Mega 80S.json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).json</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>pending,pending,pending</t>
+          <t>pending,pending</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>7cb5cb73289f21daf04426a46f283a03</t>
+          <t>c2aaf7d4be1f9bd055873ae4fea6e206</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>d7004db9de49ccecc00f0a7a18218d8d1e5914c90a80a5897f9df2aa75edc9fa,3365cbabae7349feeb66af9024ff94f1aa69ab301b375f50ec406979ab209f3b,3365cbabae7349feeb66af9024ff94f1aa69ab301b375f50ec406979ab209f3b</t>
+          <t>179121bfa9569741a3714028a4e7b3f25d0705f5d86e409039971ff6a0aeabf2, 206fabc798763a2e17c5de22364ed1088884d2926bcf51153b3af314babd7585</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>TSE enquiry (Ningbo Licheng, Mega50).pdf_197a29ce75d667e9_d7004db9de49ccec,Enquiry form - Gulf Additives (Revised 11112024).pdf_197a29ce75d667e9_3365cbabae7349fe,Enquiry_form.pdf_197a29ce75d667e9_3365cbabae7349fe</t>
+          <t>TSE Enquiry form-Mega 80S.pdf_197c45252cdeeb84_179121bfa9569741, QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf_197c45252cdeeb84_206fabc798763a2e</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>ENQUIRY</t>
+          <t>QUOTATION</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -651,109 +651,11 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>completed,completed,completed</t>
+          <t>completed,completed</t>
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Re: Submission of Enquiry Form for Co-Rotating Twin Screw Extruder</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1979b5cb8f89d5a3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>197942b8ac9cda42</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Imranshariff H S &lt;imranshariffhs@gmail.com&gt;</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45837.7861574074</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>45837.7861574074</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>45837.7861574074</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>45837.7861574074</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>enquiry_20250629_185204_EM19335_Quotation_with_material__23.05.2025.pdf</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/enquiry_20250629_185204_EM19335_Quotation_with_material__23.05.2025.pdf</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/enquiry_20250629_185204_EM19335_Quotation_with_material__23.05.2025.json</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>7fb5e4ec0bfde1feba225b6f3bdb41ab</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>564cafbe250c1903eafdd93220bef6046241b9bc14f2fa7e1a81c54ff72ef184</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>EM19335_Quotation_with_material__23.05.2025.pdf_1979b5cb8f89d5a3_564cafbe250c1903</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>downloaded</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>ENQUIRY</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>unique</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove sensitive files and update logic with Ruff linting
</commit_message>
<xml_diff>
--- a/download_email/email_download_log.xlsx
+++ b/download_email/email_download_log.xlsx
@@ -581,16 +581,16 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45839.54337962963</v>
+        <v>45840.37710648148</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45839.54337962963</v>
+        <v>45840.37710648148</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45839.54337962963</v>
+        <v>45840.37710648148</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45839.54337962963</v>
+        <v>45840.37710648148</v>
       </c>
       <c r="I2" t="n">
         <v>2</v>
@@ -600,18 +600,18 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>quotation_20250701_130227_TSE Enquiry form-Mega 80S.pdf, quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
+          <t>quotation_20250702_090301_TSE Enquiry form-Mega 80S.pdf, quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250701_130227_TSE Enquiry form-Mega 80S.pdf, /mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250702_090301_TSE Enquiry form-Mega 80S.pdf, /mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250701_130227_TSE Enquiry form-Mega 80S.json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250701_130228_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).json</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250702_090301_TSE Enquiry form-Mega 80S.json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).json</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">

</xml_diff>

<commit_message>
Fix: Ruff auto-formatting + WIP changes
</commit_message>
<xml_diff>
--- a/download_email/email_download_log.xlsx
+++ b/download_email/email_download_log.xlsx
@@ -567,30 +567,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>197c45252cdeeb84</t>
+          <t>197d02c0a64f0720</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>197c45252cdeeb84</t>
+          <t>197d02c0a64f0720</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Kumar &lt;kum4r18@gmail.com&gt;</t>
+          <t>imran shariff &lt;imran7892932345@gmail.com&gt;</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45840.37710648148</v>
+        <v>45841.53403935185</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45840.37710648148</v>
+        <v>45841.53403935185</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45840.37710648148</v>
+        <v>45841.53403935185</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45840.37710648148</v>
+        <v>45841.53403935185</v>
       </c>
       <c r="I2" t="n">
         <v>2</v>
@@ -600,18 +600,18 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>quotation_20250702_090301_TSE Enquiry form-Mega 80S.pdf, quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
+          <t>quotation_20250703_124900_TSE Enquiry form-Mega 80S.pdf, quotation_20250703_124901_B - 083 05.05.2025.pdf</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250702_090301_TSE Enquiry form-Mega 80S.pdf, /mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250703_124900_TSE Enquiry form-Mega 80S.pdf, /mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/download_email/quotation_20250703_124901_B - 083 05.05.2025.pdf</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250702_090301_TSE Enquiry form-Mega 80S.json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250702_090302_QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).json</t>
+          <t>/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250703_124900_TSE Enquiry form-Mega 80S.json,/mnt/c/Users/Imran/OneDrive - Ahana Systems and Solutions (P) Ltd/Desktop/Demo/steer_document_processing_poc/demo_app/backend/Agent_AI/result_json/quotation_20250703_124901_B - 083 05.05.2025.json</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -621,17 +621,17 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>c2aaf7d4be1f9bd055873ae4fea6e206</t>
+          <t>def4957adf44e619cfb24a4862e8f99c</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>179121bfa9569741a3714028a4e7b3f25d0705f5d86e409039971ff6a0aeabf2, 206fabc798763a2e17c5de22364ed1088884d2926bcf51153b3af314babd7585</t>
+          <t>179121bfa9569741a3714028a4e7b3f25d0705f5d86e409039971ff6a0aeabf2, 4ec14860b08a9a79e5c7bea8da7731b85d60609e6b0f3d5e1b2897e4a41e21c4</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>TSE Enquiry form-Mega 80S.pdf_197c45252cdeeb84_179121bfa9569741, QU-IMM-Vi-42025-00169-1-28-04-2025-STEER ENGG(REV).pdf_197c45252cdeeb84_206fabc798763a2e</t>
+          <t>TSE Enquiry form-Mega 80S.pdf_197d02c0a64f0720_179121bfa9569741, B - 083 05.05.2025.pdf_197d02c0a64f0720_4ec14860b08a9a79</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">

</xml_diff>